<commit_message>
burn variation through move 8
</commit_message>
<xml_diff>
--- a/Database/Openings/File-Status.xlsx
+++ b/Database/Openings/File-Status.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="107">
   <si>
     <t>Player</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Done*</t>
+  </si>
+  <si>
+    <t>E:\Chess\Database\Openings\French-Defense\French-Burn.pgn</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -676,7 +679,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,6 +876,15 @@
       <c r="C12" t="s">
         <v>95</v>
       </c>
+      <c r="D12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
finished French first 8 moves
</commit_message>
<xml_diff>
--- a/Database/Openings/File-Status.xlsx
+++ b/Database/Openings/File-Status.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="110">
   <si>
     <t>Player</t>
   </si>
@@ -340,6 +341,15 @@
   </si>
   <si>
     <t>E:\Chess\Database\Openings\French-Defense\French-Burn.pgn</t>
+  </si>
+  <si>
+    <t>E:\Chess\Database\Openings\French-Defense\French-MacCutcheon.pgn</t>
+  </si>
+  <si>
+    <t>E:\Chess\Database\Openings\French-Defense\French-Classical.pgn</t>
+  </si>
+  <si>
+    <t>E:\Chess\Database\Openings\French-Defense\French-Winawer.pgn</t>
   </si>
 </sst>
 </file>
@@ -667,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -679,7 +689,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,6 +906,15 @@
       <c r="C13" t="s">
         <v>96</v>
       </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -907,6 +926,15 @@
       <c r="C14" t="s">
         <v>97</v>
       </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -917,6 +945,15 @@
       </c>
       <c r="C15" t="s">
         <v>98</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1526,4 +1563,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished early work on 2 knights, made training file
</commit_message>
<xml_diff>
--- a/Database/Openings/File-Status.xlsx
+++ b/Database/Openings/File-Status.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\chess\Database\Openings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="112">
   <si>
     <t>Player</t>
   </si>
@@ -358,6 +353,9 @@
   </si>
   <si>
     <t>E:\Chess\Database\Openings\Caro-Kann-Exchange-Variation.pgn</t>
+  </si>
+  <si>
+    <t>E:\Chess\Database\Openings\Open-Games-e4-e5\Two-Knights-Main-Line-7...Bc5.pgn</t>
   </si>
 </sst>
 </file>
@@ -685,7 +683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -697,16 +695,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="35.875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -793,8 +791,11 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>76</v>
+      <c r="E5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -806,6 +807,15 @@
       </c>
       <c r="C6" t="s">
         <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>